<commit_message>
Se crea encuestas en bd desde excel
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="divisiónTerritorial" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="divisiónServicios" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Usuarios" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Encuestas" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mandarEncuesta" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Encuestas" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="85">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -196,18 +197,66 @@
     <t xml:space="preserve">DivisionServicios</t>
   </si>
   <si>
+    <t xml:space="preserve">Raul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tornel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saymon_set@homail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presidencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moreno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ejecutivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kike </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dallalonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gonzalez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oficinista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bravo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacheco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gisela</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simon Alberto</t>
   </si>
   <si>
     <t xml:space="preserve">Rodriguez Pacheco</t>
   </si>
   <si>
-    <t xml:space="preserve">saymon_set@homail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turista</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solangel Teresa</t>
   </si>
   <si>
@@ -217,9 +266,6 @@
     <t xml:space="preserve">Sami</t>
   </si>
   <si>
-    <t xml:space="preserve">Moreno</t>
-  </si>
-  <si>
     <t xml:space="preserve">samiraturca@hotmail.co</t>
   </si>
   <si>
@@ -229,55 +275,10 @@
     <t xml:space="preserve">Elena </t>
   </si>
   <si>
-    <t xml:space="preserve">Dallalonga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tornel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presidencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valentina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ejecutivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kike </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gonzalez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oficinista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bravo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacheco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gisela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archivo de la Encuesta </t>
+    <t xml:space="preserve">Encuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survey.json</t>
   </si>
 </sst>
 </file>
@@ -293,6 +294,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,6 +310,65 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -315,31 +376,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -347,50 +384,28 @@
       <color rgb="FF0000EE"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -398,6 +413,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -405,44 +421,22 @@
       <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFF6F9D4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -464,6 +458,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFF6F9D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
         <bgColor rgb="FF808080"/>
       </patternFill>
@@ -477,13 +495,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF38"/>
-        <bgColor rgb="FFFFF200"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF38"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -535,112 +547,96 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,24 +648,24 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
-    <cellStyle name="Normal 2" xfId="37"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Normal 2" xfId="33"/>
+    <cellStyle name="Note 7" xfId="34"/>
+    <cellStyle name="Status 10" xfId="35"/>
+    <cellStyle name="Text 6" xfId="36"/>
+    <cellStyle name="Warning 14" xfId="37"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -678,7 +674,7 @@
       <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -699,7 +695,7 @@
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF38"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -741,18 +737,20 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,11 +885,13 @@
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="26.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,10 +1144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1155,6 +1155,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.82"/>
@@ -1162,7 +1163,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,10 +1201,10 @@
         <v>60</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,59 +1212,59 @@
         <v>61</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>39</v>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>41</v>
+        <v>63</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1276,198 +1278,91 @@
         <v>59</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="saymon_set@homail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="solelena@hotmail.de"/>
-    <hyperlink ref="C4" r:id="rId3" display="samiraturca@hotmail.co"/>
+    <hyperlink ref="C3" r:id="rId2" display="saymon_set@homail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="saymon_set@homail.com"/>
     <hyperlink ref="C5" r:id="rId4" display="saymon_set@homail.com"/>
     <hyperlink ref="C6" r:id="rId5" display="saymon_set@homail.com"/>
-    <hyperlink ref="C8" r:id="rId6" display="saymon_set@homail.com"/>
-    <hyperlink ref="C9" r:id="rId7" display="saymon_set@homail.com"/>
-    <hyperlink ref="C10" r:id="rId8" display="saymon_set@homail.com"/>
-    <hyperlink ref="C11" r:id="rId9" display="saymon_set@homail.com"/>
-    <hyperlink ref="C12" r:id="rId10" display="saymon_set@homail.com"/>
-    <hyperlink ref="C13" r:id="rId11" display="saymon_set@homail.com"/>
-    <hyperlink ref="C14" r:id="rId12" display="saymon_set@homail.com"/>
-    <hyperlink ref="C15" r:id="rId13" display="saymon_set@homail.com"/>
+    <hyperlink ref="C7" r:id="rId6" display="saymon_set@homail.com"/>
+    <hyperlink ref="C8" r:id="rId7" display="saymon_set@homail.com"/>
+    <hyperlink ref="C9" r:id="rId8" display="saymon_set@homail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1484,16 +1379,160 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.22"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="saymon_set@homail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="solelena@hotmail.de"/>
+    <hyperlink ref="C4" r:id="rId3" display="samiraturca@hotmail.co"/>
+    <hyperlink ref="C5" r:id="rId4" display="saymon_set@homail.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="saymon_set@homail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,8 +1542,8 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>84</v>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,6 +1553,9 @@
       <c r="B2" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -1522,6 +1564,9 @@
       <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -1530,6 +1575,9 @@
       <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -1538,6 +1586,9 @@
       <c r="B5" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -1546,6 +1597,9 @@
       <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -1554,6 +1608,9 @@
       <c r="B7" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -1562,6 +1619,9 @@
       <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
@@ -1570,13 +1630,30 @@
       <c r="B9" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="C9" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,7 +1661,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,7 +1672,10 @@
         <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1683,10 @@
         <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1694,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1705,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,23 +1716,32 @@
         <v>18</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,7 +1749,10 @@
         <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,7 +1760,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1771,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,7 +1782,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1793,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,26 +1804,12 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C25" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Leo la encuesta desde surveyfrontend
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -11,8 +11,8 @@
     <sheet name="divisiónTerritorial" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="divisiónServicios" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Usuarios" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="mandarEncuesta" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Encuestas" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Encuestas" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mandarEncuesta" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="112">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -251,6 +251,87 @@
     <t xml:space="preserve">Gisela</t>
   </si>
   <si>
+    <t xml:space="preserve">codigoEncuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survey.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coche-24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simon Alberto</t>
   </si>
   <si>
@@ -260,25 +341,25 @@
     <t xml:space="preserve">Solangel Teresa</t>
   </si>
   <si>
-    <t xml:space="preserve">solelena@hotmail.de</t>
+    <t xml:space="preserve">oraclefedora@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sami</t>
   </si>
   <si>
-    <t xml:space="preserve">samiraturca@hotmail.co</t>
+    <t xml:space="preserve">oraclefedora@gmail.com1</t>
   </si>
   <si>
     <t xml:space="preserve">Jesus</t>
   </si>
   <si>
+    <t xml:space="preserve">2saymon_set@homail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elena </t>
   </si>
   <si>
-    <t xml:space="preserve">Encuestas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">survey.json</t>
+    <t xml:space="preserve">saymon_set@homail.com4</t>
   </si>
 </sst>
 </file>
@@ -294,7 +375,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -312,11 +392,68 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -324,88 +461,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -413,7 +480,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -421,14 +487,12 @@
       <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -437,6 +501,30 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFF6F9D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -454,30 +542,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFF6F9D4"/>
       </patternFill>
     </fill>
     <fill>
@@ -523,7 +587,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="38">
+  <cellStyleXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,50 +611,101 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -599,11 +714,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,44 +743,49 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="41">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 1 17" xfId="20"/>
-    <cellStyle name="Accent 16" xfId="21"/>
-    <cellStyle name="Accent 2 18" xfId="22"/>
-    <cellStyle name="Accent 3 19" xfId="23"/>
-    <cellStyle name="Bad 13" xfId="24"/>
-    <cellStyle name="Error 15" xfId="25"/>
-    <cellStyle name="Footnote 8" xfId="26"/>
-    <cellStyle name="Good 11" xfId="27"/>
-    <cellStyle name="Heading 1 4" xfId="28"/>
-    <cellStyle name="Heading 2 5" xfId="29"/>
-    <cellStyle name="Heading 3" xfId="30"/>
-    <cellStyle name="Hyperlink 9" xfId="31"/>
-    <cellStyle name="Neutral 12" xfId="32"/>
-    <cellStyle name="Normal 2" xfId="33"/>
-    <cellStyle name="Note 7" xfId="34"/>
-    <cellStyle name="Status 10" xfId="35"/>
-    <cellStyle name="Text 6" xfId="36"/>
-    <cellStyle name="Warning 14" xfId="37"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="37"/>
+    <cellStyle name="Accent 16" xfId="38"/>
+    <cellStyle name="Accent 2 18" xfId="39"/>
+    <cellStyle name="Accent 3 19" xfId="40"/>
+    <cellStyle name="Bad 13" xfId="41"/>
+    <cellStyle name="Error 15" xfId="42"/>
+    <cellStyle name="Footnote 8" xfId="43"/>
+    <cellStyle name="Good 11" xfId="44"/>
+    <cellStyle name="Heading 1 4" xfId="45"/>
+    <cellStyle name="Heading 2 5" xfId="46"/>
+    <cellStyle name="Heading 3" xfId="47"/>
+    <cellStyle name="Hyperlink 9" xfId="48"/>
+    <cellStyle name="Neutral 12" xfId="49"/>
+    <cellStyle name="Normal 2" xfId="50"/>
+    <cellStyle name="Note 7" xfId="51"/>
+    <cellStyle name="Status 10" xfId="52"/>
+    <cellStyle name="Text 6" xfId="53"/>
+    <cellStyle name="Warning 14" xfId="54"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -737,20 +857,20 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,19 +999,19 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="26.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,25 +1044,25 @@
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -950,25 +1070,25 @@
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -976,25 +1096,25 @@
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1002,25 +1122,25 @@
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1028,25 +1148,25 @@
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1054,25 +1174,25 @@
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1080,25 +1200,25 @@
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1106,25 +1226,25 @@
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1147,7 +1267,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1155,7 +1275,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.82"/>
@@ -1164,7 +1284,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,19 +1308,19 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1208,19 +1328,19 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1228,122 +1348,122 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1379,132 +1499,372 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="25.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="D19" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>37</v>
+      <c r="C22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="saymon_set@homail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="solelena@hotmail.de"/>
-    <hyperlink ref="C4" r:id="rId3" display="samiraturca@hotmail.co"/>
-    <hyperlink ref="C5" r:id="rId4" display="saymon_set@homail.com"/>
-    <hyperlink ref="C6" r:id="rId5" display="saymon_set@homail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1520,298 +1880,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>84</v>
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>84</v>
+      <c r="A3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>84</v>
+      <c r="A4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>84</v>
+      <c r="A5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>84</v>
+      <c r="A6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D7" s="3"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="saymon_set@homail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="oraclefedora@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="oraclefedora@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId4" display="2saymon_set@homail.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="saymon_set@homail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Se comporta la busqueda del net promoter score bien
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -856,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,7 +998,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1501,7 +1501,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1756,7 +1756,7 @@
         <v>94</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>37</v>
@@ -1773,7 +1773,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>78</v>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Seguridad con token jwt
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -12,7 +12,8 @@
     <sheet name="divisiónServicios" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Usuarios" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Encuestas" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="mandarEncuesta" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="company" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="mandarEncuesta" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="110">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -330,6 +331,18 @@
   </si>
   <si>
     <t xml:space="preserve">Coche-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun Sol</t>
   </si>
   <si>
     <t xml:space="preserve">Simon Alberto</t>
@@ -1879,10 +1892,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.22"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1910,10 +1968,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>59</v>
@@ -1924,13 +1982,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
carga las enuestas por codigo de empresas
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="divisiónTerritorial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="111">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rodriguez Pacheco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saymon_set@hotmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Solangel Teresa</t>
@@ -1894,8 +1897,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1939,8 +1942,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1974,7 +1977,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>95</v>
@@ -1982,13 +1985,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>94</v>
@@ -2002,7 +2005,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="saymon_set@homail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="saymon_set@hotmail.com"/>
     <hyperlink ref="C3" r:id="rId2" display="oraclefedora@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Multiples empresas a traves de su email
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="divisiónTerritorial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="112">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -339,19 +339,22 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
     <t xml:space="preserve">E0001</t>
   </si>
   <si>
     <t xml:space="preserve">Sun Sol</t>
   </si>
   <si>
+    <t xml:space="preserve">saymon_set@hotmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simon Alberto</t>
   </si>
   <si>
     <t xml:space="preserve">Rodriguez Pacheco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saymon_set@hotmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Solangel Teresa</t>
@@ -1895,16 +1898,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,17 +1917,26 @@
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="saymon_set@hotmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1942,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1971,13 +1983,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>95</v>
@@ -1985,13 +1997,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>94</v>

</xml_diff>